<commit_message>
edit database, clo, delete course_clo - course_plo
</commit_message>
<xml_diff>
--- a/DataForTest/CLO_Com_316101_65.xlsx
+++ b/DataForTest/CLO_Com_316101_65.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phans\Desktop\DataForTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\intern\PLOCLO_latest\DataForTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB5C890-9109-414C-B8E9-17B23AE36DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="14196" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,9 +212,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,7 +249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,7 +284,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,11 +457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>